<commit_message>
Improve the text block above the budget summary worksheet.
</commit_message>
<xml_diff>
--- a/AdministrativeBudget.xlsx
+++ b/AdministrativeBudget.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>AdministrativeBudget</t>
   </si>
   <si>
-    <t>Version: 1.1.0</t>
+    <t>Version: 1.1.1</t>
   </si>
   <si>
     <t>This spreadsheet was created by the Trustees of the Brittany, Tokai Villas Body Corporate to</t>
@@ -194,7 +194,13 @@
     <t>Budget Summary</t>
   </si>
   <si>
-    <t>A worksheet that summarizes the details of the administrative budget.</t>
+    <t>A worksheet that summarizes the details of the administrative budget. This summary shows the</t>
+  </si>
+  <si>
+    <t>anticipated percentage change in each category from the previous financial year and each</t>
+  </si>
+  <si>
+    <t>category's contribution to the overall administrative budget.</t>
   </si>
   <si>
     <t>Total administrative budget</t>
@@ -6060,10 +6066,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6084,6 +6090,8 @@
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -6092,193 +6100,171 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="str">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26" t="str">
         <f aca="false">IF('Previous Year Financials'!$B$13&lt;&gt;"Yes", "The " &amp;'Previous Year Financials'!$B$14 &amp; " figures had not been audited when the budget was prepared.", "")</f>
         <v>The 2017 figures had not been audited when the budget was prepared.</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="28" t="n">
-        <f aca="false">'Budget Planner'!D74</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="28" t="n">
-        <f aca="false">'Budget Planner'!C74</f>
-        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="25" t="e">
-        <f aca="false">B8/B9-1</f>
+      <c r="B10" s="28" t="n">
+        <f aca="false">'Budget Planner'!D74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="28" t="n">
+        <f aca="false">'Budget Planner'!C74</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="25" t="e">
+        <f aca="false">B10/B11-1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="14" t="str">
+      <c r="C15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="14" t="str">
         <f aca="false">("Change from " &amp;'Previous Year Financials'!B14)</f>
         <v>Change from 2017</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="str">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="30" t="str">
         <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I17)</f>
         <v>Repairs and Maintenance</v>
       </c>
-      <c r="B14" s="31" t="n">
+      <c r="B16" s="31" t="n">
         <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I17)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="32" t="e">
-        <f aca="false">B14/$B$8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I17)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="32" t="str">
-        <f aca="false">IF(B14&lt;&gt;0,IF(E14&lt;&gt;0,B14/E14-1,""),"")</f>
-        <v/>
-      </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I18)</f>
-        <v>0</v>
-      </c>
-      <c r="B15" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I18)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="32" t="e">
-        <f aca="false">B15/$B$8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I18)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="32" t="str">
-        <f aca="false">IF(B15&lt;&gt;0,IF(E15&lt;&gt;0,B15/E15-1,""),"")</f>
-        <v/>
-      </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I19)</f>
-        <v>0</v>
-      </c>
-      <c r="B16" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I19)</f>
-        <v>0</v>
-      </c>
       <c r="C16" s="32" t="e">
-        <f aca="false">B16/$B$8</f>
+        <f aca="false">B16/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D16" s="30"/>
       <c r="E16" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I19)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I17)</f>
         <v>0</v>
       </c>
       <c r="F16" s="32" t="str">
         <f aca="false">IF(B16&lt;&gt;0,IF(E16&lt;&gt;0,B16/E16-1,""),"")</f>
         <v/>
       </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I20)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I18)</f>
         <v>0</v>
       </c>
       <c r="B17" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I20)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I18)</f>
         <v>0</v>
       </c>
       <c r="C17" s="32" t="e">
-        <f aca="false">B17/$B$8</f>
+        <f aca="false">B17/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D17" s="30"/>
       <c r="E17" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I20)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I18)</f>
         <v>0</v>
       </c>
       <c r="F17" s="32" t="str">
         <f aca="false">IF(B17&lt;&gt;0,IF(E17&lt;&gt;0,B17/E17-1,""),"")</f>
         <v/>
       </c>
+      <c r="G17" s="26"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I21)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I19)</f>
         <v>0</v>
       </c>
       <c r="B18" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I21)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I19)</f>
         <v>0</v>
       </c>
       <c r="C18" s="32" t="e">
-        <f aca="false">B18/$B$8</f>
+        <f aca="false">B18/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I21)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I19)</f>
         <v>0</v>
       </c>
       <c r="F18" s="32" t="str">
@@ -6288,20 +6274,20 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I22)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I20)</f>
         <v>0</v>
       </c>
       <c r="B19" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I22)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I20)</f>
         <v>0</v>
       </c>
       <c r="C19" s="32" t="e">
-        <f aca="false">B19/$B$8</f>
+        <f aca="false">B19/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D19" s="30"/>
       <c r="E19" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I22)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I20)</f>
         <v>0</v>
       </c>
       <c r="F19" s="32" t="str">
@@ -6311,20 +6297,20 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I23)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I21)</f>
         <v>0</v>
       </c>
       <c r="B20" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I23)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I21)</f>
         <v>0</v>
       </c>
       <c r="C20" s="32" t="e">
-        <f aca="false">B20/$B$8</f>
+        <f aca="false">B20/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I23)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I21)</f>
         <v>0</v>
       </c>
       <c r="F20" s="32" t="str">
@@ -6334,20 +6320,20 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I24)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I22)</f>
         <v>0</v>
       </c>
       <c r="B21" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I24)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I22)</f>
         <v>0</v>
       </c>
       <c r="C21" s="32" t="e">
-        <f aca="false">B21/$B$8</f>
+        <f aca="false">B21/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D21" s="30"/>
       <c r="E21" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I24)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I22)</f>
         <v>0</v>
       </c>
       <c r="F21" s="32" t="str">
@@ -6357,20 +6343,20 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I25)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I23)</f>
         <v>0</v>
       </c>
       <c r="B22" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I25)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I23)</f>
         <v>0</v>
       </c>
       <c r="C22" s="32" t="e">
-        <f aca="false">B22/$B$8</f>
+        <f aca="false">B22/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I25)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I23)</f>
         <v>0</v>
       </c>
       <c r="F22" s="32" t="str">
@@ -6380,20 +6366,20 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I26)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I24)</f>
         <v>0</v>
       </c>
       <c r="B23" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I26)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I24)</f>
         <v>0</v>
       </c>
       <c r="C23" s="32" t="e">
-        <f aca="false">B23/$B$8</f>
+        <f aca="false">B23/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I26)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I24)</f>
         <v>0</v>
       </c>
       <c r="F23" s="32" t="str">
@@ -6403,20 +6389,20 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I27)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I25)</f>
         <v>0</v>
       </c>
       <c r="B24" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I27)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I25)</f>
         <v>0</v>
       </c>
       <c r="C24" s="32" t="e">
-        <f aca="false">B24/$B$8</f>
+        <f aca="false">B24/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I27)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I25)</f>
         <v>0</v>
       </c>
       <c r="F24" s="32" t="str">
@@ -6426,20 +6412,20 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I28)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I26)</f>
         <v>0</v>
       </c>
       <c r="B25" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I28)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I26)</f>
         <v>0</v>
       </c>
       <c r="C25" s="32" t="e">
-        <f aca="false">B25/$B$8</f>
+        <f aca="false">B25/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I28)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I26)</f>
         <v>0</v>
       </c>
       <c r="F25" s="32" t="str">
@@ -6449,20 +6435,20 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I29)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I27)</f>
         <v>0</v>
       </c>
       <c r="B26" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I29)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I27)</f>
         <v>0</v>
       </c>
       <c r="C26" s="32" t="e">
-        <f aca="false">B26/$B$8</f>
+        <f aca="false">B26/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D26" s="30"/>
       <c r="E26" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I29)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I27)</f>
         <v>0</v>
       </c>
       <c r="F26" s="32" t="str">
@@ -6472,20 +6458,20 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I30)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I28)</f>
         <v>0</v>
       </c>
       <c r="B27" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I30)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I28)</f>
         <v>0</v>
       </c>
       <c r="C27" s="32" t="e">
-        <f aca="false">B27/$B$8</f>
+        <f aca="false">B27/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D27" s="30"/>
       <c r="E27" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I30)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I28)</f>
         <v>0</v>
       </c>
       <c r="F27" s="32" t="str">
@@ -6495,20 +6481,20 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I31)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I29)</f>
         <v>0</v>
       </c>
       <c r="B28" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I31)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I29)</f>
         <v>0</v>
       </c>
       <c r="C28" s="32" t="e">
-        <f aca="false">B28/$B$8</f>
+        <f aca="false">B28/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I31)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I29)</f>
         <v>0</v>
       </c>
       <c r="F28" s="32" t="str">
@@ -6518,20 +6504,20 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I32)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I30)</f>
         <v>0</v>
       </c>
       <c r="B29" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I32)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I30)</f>
         <v>0</v>
       </c>
       <c r="C29" s="32" t="e">
-        <f aca="false">B29/$B$8</f>
+        <f aca="false">B29/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D29" s="30"/>
       <c r="E29" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I32)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I30)</f>
         <v>0</v>
       </c>
       <c r="F29" s="32" t="str">
@@ -6541,20 +6527,20 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I33)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I31)</f>
         <v>0</v>
       </c>
       <c r="B30" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I33)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I31)</f>
         <v>0</v>
       </c>
       <c r="C30" s="32" t="e">
-        <f aca="false">B30/$B$8</f>
+        <f aca="false">B30/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D30" s="30"/>
       <c r="E30" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I33)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I31)</f>
         <v>0</v>
       </c>
       <c r="F30" s="32" t="str">
@@ -6564,20 +6550,20 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I34)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I32)</f>
         <v>0</v>
       </c>
       <c r="B31" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I34)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I32)</f>
         <v>0</v>
       </c>
       <c r="C31" s="32" t="e">
-        <f aca="false">B31/$B$8</f>
+        <f aca="false">B31/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D31" s="30"/>
       <c r="E31" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I34)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I32)</f>
         <v>0</v>
       </c>
       <c r="F31" s="32" t="str">
@@ -6587,20 +6573,20 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I35)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I33)</f>
         <v>0</v>
       </c>
       <c r="B32" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I35)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I33)</f>
         <v>0</v>
       </c>
       <c r="C32" s="32" t="e">
-        <f aca="false">B32/$B$8</f>
+        <f aca="false">B32/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D32" s="30"/>
       <c r="E32" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I35)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I33)</f>
         <v>0</v>
       </c>
       <c r="F32" s="32" t="str">
@@ -6610,20 +6596,20 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I36)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I34)</f>
         <v>0</v>
       </c>
       <c r="B33" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I36)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I34)</f>
         <v>0</v>
       </c>
       <c r="C33" s="32" t="e">
-        <f aca="false">B33/$B$8</f>
+        <f aca="false">B33/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I36)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I34)</f>
         <v>0</v>
       </c>
       <c r="F33" s="32" t="str">
@@ -6633,20 +6619,20 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I37)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I35)</f>
         <v>0</v>
       </c>
       <c r="B34" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I37)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I35)</f>
         <v>0</v>
       </c>
       <c r="C34" s="32" t="e">
-        <f aca="false">B34/$B$8</f>
+        <f aca="false">B34/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I37)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I35)</f>
         <v>0</v>
       </c>
       <c r="F34" s="32" t="str">
@@ -6656,20 +6642,20 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I38)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I36)</f>
         <v>0</v>
       </c>
       <c r="B35" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I38)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I36)</f>
         <v>0</v>
       </c>
       <c r="C35" s="32" t="e">
-        <f aca="false">B35/$B$8</f>
+        <f aca="false">B35/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I38)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I36)</f>
         <v>0</v>
       </c>
       <c r="F35" s="32" t="str">
@@ -6679,20 +6665,20 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I39)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I37)</f>
         <v>0</v>
       </c>
       <c r="B36" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I39)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I37)</f>
         <v>0</v>
       </c>
       <c r="C36" s="32" t="e">
-        <f aca="false">B36/$B$8</f>
+        <f aca="false">B36/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I39)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I37)</f>
         <v>0</v>
       </c>
       <c r="F36" s="32" t="str">
@@ -6702,20 +6688,20 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I40)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I38)</f>
         <v>0</v>
       </c>
       <c r="B37" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I40)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I38)</f>
         <v>0</v>
       </c>
       <c r="C37" s="32" t="e">
-        <f aca="false">B37/$B$8</f>
+        <f aca="false">B37/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I40)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I38)</f>
         <v>0</v>
       </c>
       <c r="F37" s="32" t="str">
@@ -6725,20 +6711,20 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I41)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I39)</f>
         <v>0</v>
       </c>
       <c r="B38" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I41)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I39)</f>
         <v>0</v>
       </c>
       <c r="C38" s="32" t="e">
-        <f aca="false">B38/$B$8</f>
+        <f aca="false">B38/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I41)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I39)</f>
         <v>0</v>
       </c>
       <c r="F38" s="32" t="str">
@@ -6748,20 +6734,20 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I42)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I40)</f>
         <v>0</v>
       </c>
       <c r="B39" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I42)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I40)</f>
         <v>0</v>
       </c>
       <c r="C39" s="32" t="e">
-        <f aca="false">B39/$B$8</f>
+        <f aca="false">B39/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I42)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I40)</f>
         <v>0</v>
       </c>
       <c r="F39" s="32" t="str">
@@ -6771,20 +6757,20 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I43)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I41)</f>
         <v>0</v>
       </c>
       <c r="B40" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I43)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I41)</f>
         <v>0</v>
       </c>
       <c r="C40" s="32" t="e">
-        <f aca="false">B40/$B$8</f>
+        <f aca="false">B40/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I43)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I41)</f>
         <v>0</v>
       </c>
       <c r="F40" s="32" t="str">
@@ -6794,20 +6780,20 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I44)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I42)</f>
         <v>0</v>
       </c>
       <c r="B41" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I44)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I42)</f>
         <v>0</v>
       </c>
       <c r="C41" s="32" t="e">
-        <f aca="false">B41/$B$8</f>
+        <f aca="false">B41/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I44)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I42)</f>
         <v>0</v>
       </c>
       <c r="F41" s="32" t="str">
@@ -6817,20 +6803,20 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I45)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I43)</f>
         <v>0</v>
       </c>
       <c r="B42" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I45)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I43)</f>
         <v>0</v>
       </c>
       <c r="C42" s="32" t="e">
-        <f aca="false">B42/$B$8</f>
+        <f aca="false">B42/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I45)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I43)</f>
         <v>0</v>
       </c>
       <c r="F42" s="32" t="str">
@@ -6840,20 +6826,20 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I46)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I44)</f>
         <v>0</v>
       </c>
       <c r="B43" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I46)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I44)</f>
         <v>0</v>
       </c>
       <c r="C43" s="32" t="e">
-        <f aca="false">B43/$B$8</f>
+        <f aca="false">B43/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I46)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I44)</f>
         <v>0</v>
       </c>
       <c r="F43" s="32" t="str">
@@ -6863,20 +6849,20 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I47)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I45)</f>
         <v>0</v>
       </c>
       <c r="B44" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I47)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I45)</f>
         <v>0</v>
       </c>
       <c r="C44" s="32" t="e">
-        <f aca="false">B44/$B$8</f>
+        <f aca="false">B44/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I47)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I45)</f>
         <v>0</v>
       </c>
       <c r="F44" s="32" t="str">
@@ -6886,20 +6872,20 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I48)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I46)</f>
         <v>0</v>
       </c>
       <c r="B45" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I48)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I46)</f>
         <v>0</v>
       </c>
       <c r="C45" s="32" t="e">
-        <f aca="false">B45/$B$8</f>
+        <f aca="false">B45/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I48)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I46)</f>
         <v>0</v>
       </c>
       <c r="F45" s="32" t="str">
@@ -6909,20 +6895,20 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I49)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I47)</f>
         <v>0</v>
       </c>
       <c r="B46" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I49)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I47)</f>
         <v>0</v>
       </c>
       <c r="C46" s="32" t="e">
-        <f aca="false">B46/$B$8</f>
+        <f aca="false">B46/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I49)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I47)</f>
         <v>0</v>
       </c>
       <c r="F46" s="32" t="str">
@@ -6932,20 +6918,20 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I50)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I48)</f>
         <v>0</v>
       </c>
       <c r="B47" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I50)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I48)</f>
         <v>0</v>
       </c>
       <c r="C47" s="32" t="e">
-        <f aca="false">B47/$B$8</f>
+        <f aca="false">B47/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I50)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I48)</f>
         <v>0</v>
       </c>
       <c r="F47" s="32" t="str">
@@ -6955,20 +6941,20 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I51)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I49)</f>
         <v>0</v>
       </c>
       <c r="B48" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I51)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I49)</f>
         <v>0</v>
       </c>
       <c r="C48" s="32" t="e">
-        <f aca="false">B48/$B$8</f>
+        <f aca="false">B48/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I51)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I49)</f>
         <v>0</v>
       </c>
       <c r="F48" s="32" t="str">
@@ -6978,20 +6964,20 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I52)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I50)</f>
         <v>0</v>
       </c>
       <c r="B49" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I52)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I50)</f>
         <v>0</v>
       </c>
       <c r="C49" s="32" t="e">
-        <f aca="false">B49/$B$8</f>
+        <f aca="false">B49/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I52)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I50)</f>
         <v>0</v>
       </c>
       <c r="F49" s="32" t="str">
@@ -7001,20 +6987,20 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I53)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I51)</f>
         <v>0</v>
       </c>
       <c r="B50" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I53)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I51)</f>
         <v>0</v>
       </c>
       <c r="C50" s="32" t="e">
-        <f aca="false">B50/$B$8</f>
+        <f aca="false">B50/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I53)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I51)</f>
         <v>0</v>
       </c>
       <c r="F50" s="32" t="str">
@@ -7024,20 +7010,20 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I54)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I52)</f>
         <v>0</v>
       </c>
       <c r="B51" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I54)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I52)</f>
         <v>0</v>
       </c>
       <c r="C51" s="32" t="e">
-        <f aca="false">B51/$B$8</f>
+        <f aca="false">B51/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I54)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I52)</f>
         <v>0</v>
       </c>
       <c r="F51" s="32" t="str">
@@ -7047,20 +7033,20 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I55)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I53)</f>
         <v>0</v>
       </c>
       <c r="B52" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I55)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I53)</f>
         <v>0</v>
       </c>
       <c r="C52" s="32" t="e">
-        <f aca="false">B52/$B$8</f>
+        <f aca="false">B52/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I55)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I53)</f>
         <v>0</v>
       </c>
       <c r="F52" s="32" t="str">
@@ -7070,20 +7056,20 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I56)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I54)</f>
         <v>0</v>
       </c>
       <c r="B53" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I56)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I54)</f>
         <v>0</v>
       </c>
       <c r="C53" s="32" t="e">
-        <f aca="false">B53/$B$8</f>
+        <f aca="false">B53/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I56)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I54)</f>
         <v>0</v>
       </c>
       <c r="F53" s="32" t="str">
@@ -7093,20 +7079,20 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I57)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I55)</f>
         <v>0</v>
       </c>
       <c r="B54" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I57)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I55)</f>
         <v>0</v>
       </c>
       <c r="C54" s="32" t="e">
-        <f aca="false">B54/$B$8</f>
+        <f aca="false">B54/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I57)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I55)</f>
         <v>0</v>
       </c>
       <c r="F54" s="32" t="str">
@@ -7116,20 +7102,20 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I58)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I56)</f>
         <v>0</v>
       </c>
       <c r="B55" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I58)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I56)</f>
         <v>0</v>
       </c>
       <c r="C55" s="32" t="e">
-        <f aca="false">B55/$B$8</f>
+        <f aca="false">B55/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D55" s="30"/>
       <c r="E55" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I58)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I56)</f>
         <v>0</v>
       </c>
       <c r="F55" s="32" t="str">
@@ -7139,20 +7125,20 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I59)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I57)</f>
         <v>0</v>
       </c>
       <c r="B56" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I59)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I57)</f>
         <v>0</v>
       </c>
       <c r="C56" s="32" t="e">
-        <f aca="false">B56/$B$8</f>
+        <f aca="false">B56/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I59)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I57)</f>
         <v>0</v>
       </c>
       <c r="F56" s="32" t="str">
@@ -7162,20 +7148,20 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I60)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I58)</f>
         <v>0</v>
       </c>
       <c r="B57" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I60)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I58)</f>
         <v>0</v>
       </c>
       <c r="C57" s="32" t="e">
-        <f aca="false">B57/$B$8</f>
+        <f aca="false">B57/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I60)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I58)</f>
         <v>0</v>
       </c>
       <c r="F57" s="32" t="str">
@@ -7185,20 +7171,20 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I61)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I59)</f>
         <v>0</v>
       </c>
       <c r="B58" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I61)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I59)</f>
         <v>0</v>
       </c>
       <c r="C58" s="32" t="e">
-        <f aca="false">B58/$B$8</f>
+        <f aca="false">B58/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I61)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I59)</f>
         <v>0</v>
       </c>
       <c r="F58" s="32" t="str">
@@ -7208,20 +7194,20 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I62)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I60)</f>
         <v>0</v>
       </c>
       <c r="B59" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I62)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I60)</f>
         <v>0</v>
       </c>
       <c r="C59" s="32" t="e">
-        <f aca="false">B59/$B$8</f>
+        <f aca="false">B59/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I62)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I60)</f>
         <v>0</v>
       </c>
       <c r="F59" s="32" t="str">
@@ -7231,20 +7217,20 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I63)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I61)</f>
         <v>0</v>
       </c>
       <c r="B60" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I63)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I61)</f>
         <v>0</v>
       </c>
       <c r="C60" s="32" t="e">
-        <f aca="false">B60/$B$8</f>
+        <f aca="false">B60/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I63)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I61)</f>
         <v>0</v>
       </c>
       <c r="F60" s="32" t="str">
@@ -7254,20 +7240,20 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I64)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I62)</f>
         <v>0</v>
       </c>
       <c r="B61" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I64)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I62)</f>
         <v>0</v>
       </c>
       <c r="C61" s="32" t="e">
-        <f aca="false">B61/$B$8</f>
+        <f aca="false">B61/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I64)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I62)</f>
         <v>0</v>
       </c>
       <c r="F61" s="32" t="str">
@@ -7277,20 +7263,20 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I65)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I63)</f>
         <v>0</v>
       </c>
       <c r="B62" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I65)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I63)</f>
         <v>0</v>
       </c>
       <c r="C62" s="32" t="e">
-        <f aca="false">B62/$B$8</f>
+        <f aca="false">B62/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I65)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I63)</f>
         <v>0</v>
       </c>
       <c r="F62" s="32" t="str">
@@ -7300,20 +7286,20 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I66)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I64)</f>
         <v>0</v>
       </c>
       <c r="B63" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I66)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I64)</f>
         <v>0</v>
       </c>
       <c r="C63" s="32" t="e">
-        <f aca="false">B63/$B$8</f>
+        <f aca="false">B63/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I66)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I64)</f>
         <v>0</v>
       </c>
       <c r="F63" s="32" t="str">
@@ -7323,20 +7309,20 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I67)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I65)</f>
         <v>0</v>
       </c>
       <c r="B64" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I67)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I65)</f>
         <v>0</v>
       </c>
       <c r="C64" s="32" t="e">
-        <f aca="false">B64/$B$8</f>
+        <f aca="false">B64/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I67)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I65)</f>
         <v>0</v>
       </c>
       <c r="F64" s="32" t="str">
@@ -7346,20 +7332,20 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I68)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I66)</f>
         <v>0</v>
       </c>
       <c r="B65" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I68)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I66)</f>
         <v>0</v>
       </c>
       <c r="C65" s="32" t="e">
-        <f aca="false">B65/$B$8</f>
+        <f aca="false">B65/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D65" s="30"/>
       <c r="E65" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I68)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I66)</f>
         <v>0</v>
       </c>
       <c r="F65" s="32" t="str">
@@ -7369,20 +7355,20 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I69)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I67)</f>
         <v>0</v>
       </c>
       <c r="B66" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I69)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I67)</f>
         <v>0</v>
       </c>
       <c r="C66" s="32" t="e">
-        <f aca="false">B66/$B$8</f>
+        <f aca="false">B66/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I69)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I67)</f>
         <v>0</v>
       </c>
       <c r="F66" s="32" t="str">
@@ -7392,20 +7378,20 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I70)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I68)</f>
         <v>0</v>
       </c>
       <c r="B67" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I70)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I68)</f>
         <v>0</v>
       </c>
       <c r="C67" s="32" t="e">
-        <f aca="false">B67/$B$8</f>
+        <f aca="false">B67/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I70)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I68)</f>
         <v>0</v>
       </c>
       <c r="F67" s="32" t="str">
@@ -7415,20 +7401,20 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I71)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I69)</f>
         <v>0</v>
       </c>
       <c r="B68" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I71)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I69)</f>
         <v>0</v>
       </c>
       <c r="C68" s="32" t="e">
-        <f aca="false">B68/$B$8</f>
+        <f aca="false">B68/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I71)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I69)</f>
         <v>0</v>
       </c>
       <c r="F68" s="32" t="str">
@@ -7438,20 +7424,20 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I72)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I70)</f>
         <v>0</v>
       </c>
       <c r="B69" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I72)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I70)</f>
         <v>0</v>
       </c>
       <c r="C69" s="32" t="e">
-        <f aca="false">B69/$B$8</f>
+        <f aca="false">B69/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I72)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I70)</f>
         <v>0</v>
       </c>
       <c r="F69" s="32" t="str">
@@ -7461,20 +7447,20 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I73)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I71)</f>
         <v>0</v>
       </c>
       <c r="B70" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I73)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I71)</f>
         <v>0</v>
       </c>
       <c r="C70" s="32" t="e">
-        <f aca="false">B70/$B$8</f>
+        <f aca="false">B70/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I73)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I71)</f>
         <v>0</v>
       </c>
       <c r="F70" s="32" t="str">
@@ -7484,20 +7470,20 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I74)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I72)</f>
         <v>0</v>
       </c>
       <c r="B71" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I74)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I72)</f>
         <v>0</v>
       </c>
       <c r="C71" s="32" t="e">
-        <f aca="false">B71/$B$8</f>
+        <f aca="false">B71/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I74)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I72)</f>
         <v>0</v>
       </c>
       <c r="F71" s="32" t="str">
@@ -7507,20 +7493,20 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I75)</f>
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I73)</f>
         <v>0</v>
       </c>
       <c r="B72" s="31" t="n">
-        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I75)</f>
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I73)</f>
         <v>0</v>
       </c>
       <c r="C72" s="32" t="e">
-        <f aca="false">B72/$B$8</f>
+        <f aca="false">B72/$B$10</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30" t="n">
-        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I75)</f>
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I73)</f>
         <v>0</v>
       </c>
       <c r="F72" s="32" t="str">
@@ -7529,27 +7515,75 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="30" t="n">
+      <c r="A73" s="30" t="n">
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I74)</f>
+        <v>0</v>
+      </c>
+      <c r="B73" s="31" t="n">
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I74)</f>
+        <v>0</v>
+      </c>
+      <c r="C73" s="32" t="e">
+        <f aca="false">B73/$B$10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30" t="n">
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I74)</f>
+        <v>0</v>
+      </c>
+      <c r="F73" s="32" t="str">
+        <f aca="false">IF(B73&lt;&gt;0,IF(E73&lt;&gt;0,B73/E73-1,""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="30" t="n">
+        <f aca="false">INDEX('Previous Year Financials'!A$17:A$202,'Previous Year Financials'!I75)</f>
+        <v>0</v>
+      </c>
+      <c r="B74" s="31" t="n">
+        <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I75)</f>
+        <v>0</v>
+      </c>
+      <c r="C74" s="32" t="e">
+        <f aca="false">B74/$B$10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30" t="n">
+        <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I75)</f>
+        <v>0</v>
+      </c>
+      <c r="F74" s="32" t="str">
+        <f aca="false">IF(B74&lt;&gt;0,IF(E74&lt;&gt;0,B74/E74-1,""),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="30" t="n">
         <f aca="false">INDEX('Budget Planner'!F$14:F$181,'Previous Year Financials'!I76)</f>
         <v>0</v>
       </c>
-      <c r="C73" s="32"/>
-      <c r="E73" s="19" t="n">
+      <c r="C75" s="32"/>
+      <c r="E75" s="19" t="n">
         <f aca="false">INDEX('Previous Year Financials'!E$17:E$186,'Previous Year Financials'!I76)</f>
         <v>0</v>
       </c>
-      <c r="F73" s="32" t="str">
-        <f aca="false">IF(B73&lt;&gt;0,B73/E73-1,"")</f>
+      <c r="F75" s="32" t="str">
+        <f aca="false">IF(B75&lt;&gt;0,B75/E75-1,"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true" selectLockedCells="true"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
+  <mergeCells count="6">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>